<commit_message>
Continue implementing concertina gait, begin moving common functionality to a shared library, add servo testing sketch
Continued implementing the concertina gait, began moving shared
functionality to a shared library ("SnakeRobotShared"), which can be
installed for the Arduino IDE manually by copying the folder to the
Arduino libraries directory or automatically on most Windows
environments via "locallibinstall.bat". A servo testing sketch was also
added to aid in various troubleshooting and other tasks (e.g. checking
servo mounting alignment, checking wiring, finding appropriate angles
for movements).
</commit_message>
<xml_diff>
--- a/Concertina Wave Calculator.xlsx
+++ b/Concertina Wave Calculator.xlsx
@@ -265,40 +265,40 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.669459319687682</c:v>
+                  <c:v>21.893654271085456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.381583263896601</c:v>
+                  <c:v>28.112825339129817</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.221480678472354</c:v>
+                  <c:v>32.85810137056923</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.267703055701546</c:v>
+                  <c:v>35.856119860652782</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.477170208095504</c:v>
+                  <c:v>37.710181059326388</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6866373604894624</c:v>
+                  <c:v>39.564242257999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.2671402622813455</c:v>
+                  <c:v>42.562260748083546</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.4272428477055934</c:v>
+                  <c:v>47.307536779522962</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.71511890349667873</c:v>
+                  <c:v>53.526707847567323</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9543404161910036</c:v>
+                  <c:v>60.420362118652776</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.954340416191004</c:v>
+                  <c:v>67.420362118652776</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.454340416191002</c:v>
+                  <c:v>78.920362118652776</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,40 +313,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1256322313681406</c:v>
+                  <c:v>1.2155372436685123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0602877245565043</c:v>
+                  <c:v>4.4283103801348833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.718662662966288</c:v>
+                  <c:v>9.5744113687909156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.40003903853475</c:v>
+                  <c:v>15.899906221616039</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.099645947670911</c:v>
+                  <c:v>22.649903041731807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.799252856807072</c:v>
+                  <c:v>29.399899861847576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.480629232375534</c:v>
+                  <c:v>35.725394714672703</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.13900417078532</c:v>
+                  <c:v>40.871495703328733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.073659663973686</c:v>
+                  <c:v>44.084268839795108</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,6 +373,8 @@
         <c:axId val="254286600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
+          <c:min val="-30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -495,6 +497,8 @@
         <c:axId val="254291520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -843,40 +847,40 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.669459319687682</c:v>
+                  <c:v>21.893654271085456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.381583263896601</c:v>
+                  <c:v>28.112825339129817</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.221480678472354</c:v>
+                  <c:v>32.85810137056923</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.267703055701546</c:v>
+                  <c:v>35.856119860652782</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.477170208095504</c:v>
+                  <c:v>37.710181059326388</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6866373604894624</c:v>
+                  <c:v>39.564242257999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.2671402622813455</c:v>
+                  <c:v>42.562260748083546</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.4272428477055934</c:v>
+                  <c:v>47.307536779522962</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.71511890349667873</c:v>
+                  <c:v>53.526707847567323</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9543404161910036</c:v>
+                  <c:v>60.420362118652776</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.954340416191004</c:v>
+                  <c:v>67.420362118652776</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.454340416191002</c:v>
+                  <c:v>78.920362118652776</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1263,40 +1267,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1256322313681406</c:v>
+                  <c:v>1.2155372436685123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0602877245565043</c:v>
+                  <c:v>4.4283103801348833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.718662662966288</c:v>
+                  <c:v>9.5744113687909156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.40003903853475</c:v>
+                  <c:v>15.899906221616039</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.099645947670911</c:v>
+                  <c:v>22.649903041731807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.799252856807072</c:v>
+                  <c:v>29.399899861847576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.480629232375534</c:v>
+                  <c:v>35.725394714672703</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.13900417078532</c:v>
+                  <c:v>40.871495703328733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.073659663973686</c:v>
+                  <c:v>44.084268839795108</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40.19929189534183</c:v>
+                  <c:v>45.299806083463622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3162,14 +3166,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>152398</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3516,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3571,10 +3575,10 @@
         <v>30</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3615,19 +3619,19 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H14" si="1">$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G3)*(ABS(G3))^($E$5+$C$8*($E$8-$E$5))</f>
-        <v>110.67766952966369</v>
+        <v>103</v>
       </c>
       <c r="I3">
         <f>I2+(H3-$B$5)</f>
-        <v>17.677669529663689</v>
+        <v>10</v>
       </c>
       <c r="J3">
         <f>J2+$A$5*COS(PI()*I3/180)</f>
-        <v>21.669459319687682</v>
+        <v>21.893654271085456</v>
       </c>
       <c r="K3">
         <f>K2+$A$5*SIN(PI()*I3/180)</f>
-        <v>2.1256322313681406</v>
+        <v>1.2155372436685123</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3656,19 +3660,19 @@
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>133.29637244338281</v>
+        <v>110.32050807568876</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I13" si="3">I3+(H4-$B$5)</f>
-        <v>57.974041973046496</v>
+        <v>27.320508075688764</v>
       </c>
       <c r="J4">
         <f>J3+$A$5*COS(PI()*I4/180)</f>
-        <v>25.381583263896601</v>
+        <v>28.112825339129817</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K13" si="4">K3+$A$5*SIN(PI()*I4/180)</f>
-        <v>8.0602877245565043</v>
+        <v>4.4283103801348833</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3697,19 +3701,19 @@
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>107.9740419730465</v>
+        <v>47.320508075688764</v>
       </c>
       <c r="J5">
         <f>J4+$A$5*COS(PI()*I5/180)</f>
-        <v>23.221480678472354</v>
+        <v>32.85810137056923</v>
       </c>
       <c r="K5">
         <f t="shared" si="4"/>
-        <v>14.718662662966288</v>
+        <v>9.5744113687909156</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3723,19 +3727,19 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>133.29637244338284</v>
+        <v>110.32050807568878</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>148.27041441642933</v>
+        <v>64.641016151377542</v>
       </c>
       <c r="J6">
         <f>J5+$A$5*COS(PI()*I6/180)</f>
-        <v>17.267703055701546</v>
+        <v>35.856119860652782</v>
       </c>
       <c r="K6">
         <f t="shared" si="4"/>
-        <v>18.40003903853475</v>
+        <v>15.899906221616039</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3755,27 +3759,27 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>110.67766952966369</v>
+        <v>103</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>165.94808394609302</v>
+        <v>74.641016151377542</v>
       </c>
       <c r="J7">
         <f t="shared" ref="J7:J12" si="5">J6+$A$5*COS(PI()*I7/180)</f>
-        <v>10.477170208095504</v>
+        <v>37.710181059326388</v>
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>20.099645947670911</v>
+        <v>22.649903041731807</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -3791,15 +3795,15 @@
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>165.94808394609302</v>
+        <v>74.641016151377542</v>
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>3.6866373604894624</v>
+        <v>39.564242257999993</v>
       </c>
       <c r="K8">
         <f t="shared" si="4"/>
-        <v>21.799252856807072</v>
+        <v>29.399899861847576</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3813,19 +3817,19 @@
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>75.322330470336311</v>
+        <v>83</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>148.27041441642933</v>
+        <v>64.641016151377542</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>-2.2671402622813455</v>
+        <v>42.562260748083546</v>
       </c>
       <c r="K9">
         <f t="shared" si="4"/>
-        <v>25.480629232375534</v>
+        <v>35.725394714672703</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3839,19 +3843,19 @@
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>52.703627556617192</v>
+        <v>75.679491924311236</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>107.97404197304652</v>
+        <v>47.320508075688778</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>-4.4272428477055934</v>
+        <v>47.307536779522962</v>
       </c>
       <c r="K10">
         <f t="shared" si="4"/>
-        <v>32.13900417078532</v>
+        <v>40.871495703328733</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3865,19 +3869,19 @@
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>57.974041973046525</v>
+        <v>27.320508075688778</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>-0.71511890349667873</v>
+        <v>53.526707847567323</v>
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>38.073659663973686</v>
+        <v>44.084268839795108</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3891,19 +3895,19 @@
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>52.703627556617185</v>
+        <v>75.679491924311236</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>17.67766952966371</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>5.9543404161910036</v>
+        <v>60.420362118652776</v>
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>40.19929189534183</v>
+        <v>45.299806083463622</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3917,7 +3921,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>75.322330470336283</v>
+        <v>82.999999999999986</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
@@ -3925,11 +3929,11 @@
       </c>
       <c r="J13">
         <f>J12+$A$5*COS(PI()*I13/180)</f>
-        <v>12.954340416191004</v>
+        <v>67.420362118652776</v>
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>40.19929189534183</v>
+        <v>45.299806083463622</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3951,29 +3955,29 @@
       </c>
       <c r="J14">
         <f>J13+$D$5*COS(PI()*I14/180)</f>
-        <v>24.454340416191002</v>
+        <v>78.920362118652776</v>
       </c>
       <c r="K14">
         <f>K13+$D$5*SIN(PI()*I14/180)</f>
-        <v>40.19929189534183</v>
+        <v>45.299806083463622</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15">
         <f>SLOPE(K2:K13, J2:J13)</f>
-        <v>-0.9129993514464364</v>
+        <v>1.0954522946757259</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>180*ATAN(M15)/PI()</f>
-        <v>-42.396058942212044</v>
+        <v>47.608141268433776</v>
       </c>
     </row>
     <row r="19" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K19">
         <f>180*ATAN(SLOPE(K2:K14, F2:F14)/SLOPE(J2:J14,F2:F14))/PI()</f>
-        <v>-73.810324517477184</v>
+        <v>44.726346401300617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix and refine concertina gait spreadsheet, continue testing concertina gait code
</commit_message>
<xml_diff>
--- a/Concertina Wave Calculator.xlsx
+++ b/Concertina Wave Calculator.xlsx
@@ -205,148 +205,104 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.26378363652564407"/>
-                  <c:y val="9.262680927099097E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$14</c:f>
+              <c:f>Sheet1!$J$2:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.893654271085456</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.112825339129817</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.85810137056923</c:v>
+                  <c:v>27.203981278266617</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.856119860652782</c:v>
+                  <c:v>27.222988917366919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.710181059326388</c:v>
+                  <c:v>22.904889870236744</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.564242257999993</c:v>
+                  <c:v>17.034449127294753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.562260748083546</c:v>
+                  <c:v>11.01660000351437</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.307536779522962</c:v>
+                  <c:v>5.3641231109128418</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53.526707847567323</c:v>
+                  <c:v>1.8909179691627664</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60.420362118652776</c:v>
+                  <c:v>3.3736368275457087</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67.420362118652776</c:v>
+                  <c:v>9.4417524502773258</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78.920362118652776</c:v>
+                  <c:v>16.367709097540981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.746066446616986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$14</c:f>
+              <c:f>Sheet1!$K$2:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2155372436685123</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4283103801348833</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5744113687909156</c:v>
+                  <c:v>4.6817281911117554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.899906221616039</c:v>
+                  <c:v>11.681702384611031</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.649903041731807</c:v>
+                  <c:v>17.191150689039841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.399899861847576</c:v>
+                  <c:v>21.004013849921265</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.725394714672703</c:v>
+                  <c:v>24.579694473720835</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.871495703328733</c:v>
+                  <c:v>28.708799095622027</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.084268839795108</c:v>
+                  <c:v>34.786368185588906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>41.627533640903927</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>45.117228869596609</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>44.101785852867266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42.433558039669059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,6 +311,292 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B6AB-4D4E-99C1-99116E3B4FD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Average Position</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14.754793935624003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>22.565254519475179</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B68-4650-B34A-E112D10E5B57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Regression Line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$22:$K$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$22:$L$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>-15.293540120834997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.6467700604174986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6467700604174986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.293540120834997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.940310181252496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.587080241669995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.23385030208749</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.880620362504992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.527390422922487</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.174160483339989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68.820930543757484</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>76.467700604174979</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84.114470664592474</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>91.761240725009984</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.408010785427479</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>107.05478084584497</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>114.70155090626247</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>122.34832096667998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>129.99509102709746</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>137.64186108751497</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>145.28863114793248</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>152.93540120834996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>160.58217126876747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>168.22894132918495</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175.87571138960246</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>183.52248145001997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>191.16925151043745</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>198.81602157085496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B68-4650-B34A-E112D10E5B57}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -373,7 +615,7 @@
         <c:axId val="254286600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="50"/>
+          <c:max val="130"/>
           <c:min val="-30"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -498,7 +740,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
-          <c:min val="0"/>
+          <c:min val="-60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -755,8 +997,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.16533092738407698"/>
-                  <c:y val="8.8425925925925929E-3"/>
+                  <c:x val="-0.29739228472729567"/>
+                  <c:y val="8.5135243511227768E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -791,10 +1033,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$14</c:f>
+              <c:f>Sheet1!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -833,54 +1075,60 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$14</c:f>
+              <c:f>Sheet1!$J$2:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.893654271085456</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.112825339129817</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.85810137056923</c:v>
+                  <c:v>27.203981278266617</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.856119860652782</c:v>
+                  <c:v>27.222988917366919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.710181059326388</c:v>
+                  <c:v>22.904889870236744</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.564242257999993</c:v>
+                  <c:v>17.034449127294753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.562260748083546</c:v>
+                  <c:v>11.01660000351437</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.307536779522962</c:v>
+                  <c:v>5.3641231109128418</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53.526707847567323</c:v>
+                  <c:v>1.8909179691627664</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60.420362118652776</c:v>
+                  <c:v>3.3736368275457087</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67.420362118652776</c:v>
+                  <c:v>9.4417524502773258</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78.920362118652776</c:v>
+                  <c:v>16.367709097540981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.746066446616986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,10 +1459,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$14</c:f>
+              <c:f>Sheet1!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1253,54 +1501,60 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$14</c:f>
+              <c:f>Sheet1!$K$2:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2155372436685123</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4283103801348833</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5744113687909156</c:v>
+                  <c:v>4.6817281911117554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.899906221616039</c:v>
+                  <c:v>11.681702384611031</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.649903041731807</c:v>
+                  <c:v>17.191150689039841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.399899861847576</c:v>
+                  <c:v>21.004013849921265</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.725394714672703</c:v>
+                  <c:v>24.579694473720835</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.871495703328733</c:v>
+                  <c:v>28.708799095622027</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.084268839795108</c:v>
+                  <c:v>34.786368185588906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>41.627533640903927</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>45.117228869596609</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.299806083463622</c:v>
+                  <c:v>44.101785852867266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42.433558039669059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3195,15 +3449,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3225,15 +3479,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3518,10 +3772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,6 +3789,7 @@
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" customWidth="1"/>
     <col min="11" max="11" width="26.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
     <col min="13" max="13" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3572,7 +3827,8 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <f>180/7</f>
+        <v>25.714285714285715</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -3581,7 +3837,7 @@
         <v>60</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>67.53994047895678</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3590,19 +3846,16 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SIN(PI()*($D$2+F2*$A$2)/180)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G2)*(ABS(G2))^($E$5+$C$8*($E$8-$E$5))</f>
         <v>93</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <f>$E$2</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3614,24 +3867,21 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G14" si="0">SIN(PI()*($D$2+F3*$A$2)/180)</f>
-        <v>0.49999999999999994</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1">$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G3)*(ABS(G3))^($E$5+$C$8*($E$8-$E$5))</f>
-        <v>103</v>
+        <f>$C$5</f>
+        <v>93</v>
       </c>
       <c r="I3">
-        <f>I2+(H3-$B$5)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f>J2+$A$5*COS(PI()*I3/180)</f>
-        <v>21.893654271085456</v>
+        <f>$E$2</f>
+        <v>15</v>
       </c>
       <c r="K3">
-        <f>K2+$A$5*SIN(PI()*I3/180)</f>
-        <v>1.2155372436685123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3651,28 +3901,27 @@
         <v>15</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F14" si="2">F3+1</f>
+        <f t="shared" ref="F4:F15" si="0">F3+1</f>
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0.8660254037844386</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>110.32050807568876</v>
+        <f>$C$5</f>
+        <v>93</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I13" si="3">I3+(H4-$B$5)</f>
-        <v>27.320508075688764</v>
+        <f>I3+(H4-$B$5)</f>
+        <v>0</v>
       </c>
       <c r="J4">
         <f>J3+$A$5*COS(PI()*I4/180)</f>
-        <v>28.112825339129817</v>
+        <v>22</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K13" si="4">K3+$A$5*SIN(PI()*I4/180)</f>
-        <v>4.4283103801348833</v>
+        <f>K3+$A$5*SIN(PI()*I4/180)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3692,54 +3941,54 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>SIN(PI()*($D$2+(F5-3)*$A$2)/180)</f>
+        <v>0.92414607390473669</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>113</v>
+        <f t="shared" ref="H5:H14" si="1">$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G5)*(ABS(G5))^($E$5+$C$8*($E$8-$E$5))</f>
+        <v>134.97592702454676</v>
       </c>
       <c r="I5">
-        <f t="shared" si="3"/>
-        <v>47.320508075688764</v>
+        <f t="shared" ref="I5:I14" si="2">I4+(H5-$B$5)</f>
+        <v>41.975927024546763</v>
       </c>
       <c r="J5">
         <f>J4+$A$5*COS(PI()*I5/180)</f>
-        <v>32.85810137056923</v>
+        <v>27.203981278266617</v>
       </c>
       <c r="K5">
-        <f t="shared" si="4"/>
-        <v>9.5744113687909156</v>
+        <f t="shared" ref="K5:K14" si="3">K4+$A$5*SIN(PI()*I5/180)</f>
+        <v>4.6817281911117554</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0.86602540378443871</v>
+        <f>SIN(PI()*($D$2+(F6-3)*$A$2)/180)</f>
+        <v>0.99838748612542505</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>110.32050807568878</v>
+        <v>140.8684931415562</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
-        <v>64.641016151377542</v>
+        <f t="shared" si="2"/>
+        <v>89.844420166102964</v>
       </c>
       <c r="J6">
         <f>J5+$A$5*COS(PI()*I6/180)</f>
-        <v>35.856119860652782</v>
+        <v>27.222988917366919</v>
       </c>
       <c r="K6">
-        <f t="shared" si="4"/>
-        <v>15.899906221616039</v>
+        <f t="shared" si="3"/>
+        <v>11.681702384611031</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3750,138 +3999,138 @@
         <v>16</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>0.49999999999999994</v>
+        <f t="shared" ref="G7:G14" si="4">SIN(PI()*($D$2+(F7-3)*$A$2)/180)</f>
+        <v>0.87488601229999619</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>131.24359775093944</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>128.08801791704241</v>
+      </c>
+      <c r="J7">
+        <f>J6+$A$5*COS(PI()*I7/180)</f>
+        <v>22.904889870236744</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="3"/>
-        <v>74.641016151377542</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ref="J7:J12" si="5">J6+$A$5*COS(PI()*I7/180)</f>
-        <v>37.710181059326388</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="4"/>
-        <v>22.649903041731807</v>
+        <v>17.191150689039841</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>1.22514845490862E-16</v>
+        <f t="shared" si="4"/>
+        <v>0.57810263396575434</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>111.90817656860636</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>146.99619448564877</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J13" si="5">J7+$A$5*COS(PI()*I8/180)</f>
+        <v>17.034449127294753</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="3"/>
-        <v>74.641016151377542</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="5"/>
-        <v>39.564242257999993</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="4"/>
-        <v>29.399899861847576</v>
+        <v>21.004013849921265</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>-0.50000000000000011</v>
+        <f t="shared" si="4"/>
+        <v>0.16681893901106776</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>95.28590585685582</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
-        <v>64.641016151377542</v>
+        <f t="shared" si="2"/>
+        <v>149.28210034250458</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>42.562260748083546</v>
+        <v>11.01660000351437</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
-        <v>35.725394714672703</v>
+        <f t="shared" si="3"/>
+        <v>24.579694473720835</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
-        <v>-0.86602540378443837</v>
+        <f t="shared" si="4"/>
+        <v>-0.27750529271478519</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>75.679491924311236</v>
+        <v>87.569967894277681</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
-        <v>47.320508075688778</v>
+        <f t="shared" si="2"/>
+        <v>143.85206823678226</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>47.307536779522962</v>
+        <v>5.3641231109128418</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
-        <v>40.871495703328733</v>
+        <f t="shared" si="3"/>
+        <v>28.708799095622027</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+        <f t="shared" si="4"/>
+        <v>-0.66686619783940693</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>68.895005601270114</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
-        <v>27.320508075688778</v>
+        <f t="shared" si="2"/>
+        <v>119.74707383805237</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>53.526707847567323</v>
+        <v>1.8909179691627664</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
-        <v>44.084268839795108</v>
+        <f t="shared" si="3"/>
+        <v>34.786368185588906</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3890,94 +4139,424 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
-        <v>-0.8660254037844386</v>
+        <f t="shared" si="4"/>
+        <v>-0.92414607390473658</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>75.679491924311236</v>
+        <v>51.024072975453265</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>10.000000000000014</v>
+        <f t="shared" si="2"/>
+        <v>77.771146813505638</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>60.420362118652776</v>
+        <v>3.3736368275457087</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
-        <v>45.299806083463622</v>
+        <f t="shared" si="3"/>
+        <v>41.627533640903927</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>-0.50000000000000044</v>
+        <f t="shared" si="4"/>
+        <v>-0.99838748612542505</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>82.999999999999986</v>
+        <v>45.131506858443792</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>29.90265367194943</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>9.4417524502773258</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f>J12+$A$5*COS(PI()*I13/180)</f>
-        <v>67.420362118652776</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="4"/>
-        <v>45.299806083463622</v>
+        <v>45.117228869596609</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
-        <v>-2.45029690981724E-16</v>
+        <f t="shared" si="4"/>
+        <v>-0.87488601229999585</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
+        <v>54.756402249060564</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-8.340944078990006</v>
+      </c>
+      <c r="J14">
+        <f>J13+$A$5*COS(PI()*I14/180)</f>
+        <v>16.367709097540981</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>44.101785852867266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>$C$5</f>
         <v>93</v>
       </c>
-      <c r="I14">
-        <f>I13+(H14-$B$5)</f>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f>J13+$D$5*COS(PI()*I14/180)</f>
-        <v>78.920362118652776</v>
-      </c>
-      <c r="K14">
-        <f>K13+$D$5*SIN(PI()*I14/180)</f>
-        <v>45.299806083463622</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>I14+(H15-$B$5)</f>
+        <v>-8.340944078990006</v>
+      </c>
+      <c r="J15">
+        <f>J14+$D$5*COS(PI()*I15/180)</f>
+        <v>27.746066446616986</v>
+      </c>
+      <c r="K15">
+        <f>K14+$D$5*SIN(PI()*I15/180)</f>
+        <v>42.433558039669059</v>
+      </c>
+      <c r="L15">
+        <f>K15/J15</f>
+        <v>1.5293540120834996</v>
+      </c>
       <c r="M15">
-        <f>SLOPE(K2:K13, J2:J13)</f>
-        <v>1.0954522946757259</v>
+        <f>SLOPE(K3:K14, J3:J14)</f>
+        <v>-1.2750929103360547</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>180*ATAN(M15)/PI()</f>
-        <v>47.608141268433776</v>
-      </c>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+        <v>-51.894450498809817</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f>AVERAGE(J2:J15)</f>
+        <v>14.754793935624003</v>
+      </c>
+      <c r="K17">
+        <f>AVERAGE(K2:K15)</f>
+        <v>22.565254519475179</v>
+      </c>
+      <c r="L17">
+        <f>K17-L15*J17</f>
+        <v>-4.8783436678689895E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K19">
-        <f>180*ATAN(SLOPE(K2:K14, F2:F14)/SLOPE(J2:J14,F2:F14))/PI()</f>
-        <v>44.726346401300617</v>
+        <f>SLOPE(K2:K15, F2:F15)/SLOPE(J2:J15,F2:F15)</f>
+        <v>-20.751888894693302</v>
+      </c>
+    </row>
+    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>-10</v>
+      </c>
+      <c r="L22">
+        <f>$L$15*K22</f>
+        <v>-15.293540120834997</v>
+      </c>
+    </row>
+    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f>K22+5</f>
+        <v>-5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L50" si="6">$L$15*K23</f>
+        <v>-7.6467700604174986</v>
+      </c>
+    </row>
+    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" ref="K24:K27" si="7">K23+5</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="6"/>
+        <v>7.6467700604174986</v>
+      </c>
+    </row>
+    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="6"/>
+        <v>15.293540120834997</v>
+      </c>
+    </row>
+    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="6"/>
+        <v>22.940310181252496</v>
+      </c>
+    </row>
+    <row r="28" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <f>K27+5</f>
+        <v>20</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="6"/>
+        <v>30.587080241669995</v>
+      </c>
+    </row>
+    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <f t="shared" ref="K29:K50" si="8">K28+5</f>
+        <v>25</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="6"/>
+        <v>38.23385030208749</v>
+      </c>
+    </row>
+    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>45.880620362504992</v>
+      </c>
+    </row>
+    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="6"/>
+        <v>53.527390422922487</v>
+      </c>
+    </row>
+    <row r="32" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="6"/>
+        <v>61.174160483339989</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="6"/>
+        <v>68.820930543757484</v>
+      </c>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="6"/>
+        <v>76.467700604174979</v>
+      </c>
+    </row>
+    <row r="35" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>84.114470664592474</v>
+      </c>
+    </row>
+    <row r="36" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>91.761240725009984</v>
+      </c>
+    </row>
+    <row r="37" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>99.408010785427479</v>
+      </c>
+    </row>
+    <row r="38" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>107.05478084584497</v>
+      </c>
+    </row>
+    <row r="39" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>114.70155090626247</v>
+      </c>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="6"/>
+        <v>122.34832096667998</v>
+      </c>
+    </row>
+    <row r="41" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f t="shared" si="8"/>
+        <v>85</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="6"/>
+        <v>129.99509102709746</v>
+      </c>
+    </row>
+    <row r="42" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="6"/>
+        <v>137.64186108751497</v>
+      </c>
+    </row>
+    <row r="43" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="6"/>
+        <v>145.28863114793248</v>
+      </c>
+    </row>
+    <row r="44" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="6"/>
+        <v>152.93540120834996</v>
+      </c>
+    </row>
+    <row r="45" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="6"/>
+        <v>160.58217126876747</v>
+      </c>
+    </row>
+    <row r="46" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <f t="shared" si="8"/>
+        <v>110</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="6"/>
+        <v>168.22894132918495</v>
+      </c>
+    </row>
+    <row r="47" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f t="shared" si="8"/>
+        <v>115</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="6"/>
+        <v>175.87571138960246</v>
+      </c>
+    </row>
+    <row r="48" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>120</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>183.52248145001997</v>
+      </c>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="6"/>
+        <v>191.16925151043745</v>
+      </c>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <f t="shared" si="8"/>
+        <v>130</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="6"/>
+        <v>198.81602157085496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement calibration for concertina gait
Implemented calibration for the concertina gait that attempts to align
the front of the head, end of the tail, and center of mass of the snake
in order to reduce turning while attempting to move in the forward or
reverse direction without turning.
</commit_message>
<xml_diff>
--- a/Concertina Wave Calculator.xlsx
+++ b/Concertina Wave Calculator.xlsx
@@ -221,37 +221,37 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.203981278266617</c:v>
+                  <c:v>28.837135435453831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.222988917366919</c:v>
+                  <c:v>35.789804910850663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.904889870236744</c:v>
+                  <c:v>41.07679494767757</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.034449127294753</c:v>
+                  <c:v>40.43838070802984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.01660000351437</c:v>
+                  <c:v>38.319883864504078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3641231109128418</c:v>
+                  <c:v>36.876530934310011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8909179691627664</c:v>
+                  <c:v>40.963007898491036</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3736368275457087</c:v>
+                  <c:v>47.963007898491036</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4417524502773258</c:v>
+                  <c:v>54.800143333944867</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.367709097540981</c:v>
+                  <c:v>61.752812809341698</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.746066446616986</c:v>
+                  <c:v>73.175055518922207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -272,37 +272,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6817281911117554</c:v>
+                  <c:v>1.5011925383712628</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.681702384611031</c:v>
+                  <c:v>2.3138346280301421</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.191150689039841</c:v>
+                  <c:v>-2.2739465732144191</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.004013849921265</c:v>
+                  <c:v>-9.2447734437237568</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.579694473720835</c:v>
+                  <c:v>-15.916502689127183</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.708799095622027</c:v>
+                  <c:v>-22.766081677568749</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.786368185588906</c:v>
+                  <c:v>-28.449452686153165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41.627533640903927</c:v>
+                  <c:v>-28.449452686153172</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45.117228869596609</c:v>
+                  <c:v>-26.948260147781916</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44.101785852867266</c:v>
+                  <c:v>-26.13561805812304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.433558039669059</c:v>
+                  <c:v>-24.800563196540597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,7 +349,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14.754793935624003</c:v>
+                  <c:v>38.356611304286915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,7 +361,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22.565254519475179</c:v>
+                  <c:v>-12.940687427998899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -504,91 +504,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>-15.293540120834997</c:v>
+                  <c:v>3.3892100280166462</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.6467700604174986</c:v>
+                  <c:v>1.6946050140083231</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6467700604174986</c:v>
+                  <c:v>-1.6946050140083231</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.293540120834997</c:v>
+                  <c:v>-3.3892100280166462</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.940310181252496</c:v>
+                  <c:v>-5.0838150420249688</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.587080241669995</c:v>
+                  <c:v>-6.7784200560332923</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.23385030208749</c:v>
+                  <c:v>-8.473025070041615</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.880620362504992</c:v>
+                  <c:v>-10.167630084049938</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53.527390422922487</c:v>
+                  <c:v>-11.86223509805826</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61.174160483339989</c:v>
+                  <c:v>-13.556840112066585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>68.820930543757484</c:v>
+                  <c:v>-15.251445126074907</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76.467700604174979</c:v>
+                  <c:v>-16.94605014008323</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>84.114470664592474</c:v>
+                  <c:v>-18.640655154091554</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.761240725009984</c:v>
+                  <c:v>-20.335260168099875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99.408010785427479</c:v>
+                  <c:v>-22.0298651821082</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>107.05478084584497</c:v>
+                  <c:v>-23.724470196116521</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>114.70155090626247</c:v>
+                  <c:v>-25.419075210124845</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>122.34832096667998</c:v>
+                  <c:v>-27.113680224133169</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>129.99509102709746</c:v>
+                  <c:v>-28.80828523814149</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>137.64186108751497</c:v>
+                  <c:v>-30.502890252149815</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>145.28863114793248</c:v>
+                  <c:v>-32.197495266158136</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>152.93540120834996</c:v>
+                  <c:v>-33.89210028016646</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>160.58217126876747</c:v>
+                  <c:v>-35.586705294174784</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>168.22894132918495</c:v>
+                  <c:v>-37.281310308183109</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>175.87571138960246</c:v>
+                  <c:v>-38.975915322191426</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>183.52248145001997</c:v>
+                  <c:v>-40.67052033619975</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>191.16925151043745</c:v>
+                  <c:v>-42.365125350208075</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>198.81602157085496</c:v>
+                  <c:v>-44.059730364216399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,37 +1098,37 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.203981278266617</c:v>
+                  <c:v>28.837135435453831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.222988917366919</c:v>
+                  <c:v>35.789804910850663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.904889870236744</c:v>
+                  <c:v>41.07679494767757</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.034449127294753</c:v>
+                  <c:v>40.43838070802984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.01660000351437</c:v>
+                  <c:v>38.319883864504078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3641231109128418</c:v>
+                  <c:v>36.876530934310011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8909179691627664</c:v>
+                  <c:v>40.963007898491036</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3736368275457087</c:v>
+                  <c:v>47.963007898491036</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4417524502773258</c:v>
+                  <c:v>54.800143333944867</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.367709097540981</c:v>
+                  <c:v>61.752812809341698</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.746066446616986</c:v>
+                  <c:v>73.175055518922207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1335,7 +1335,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1524,37 +1523,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6817281911117554</c:v>
+                  <c:v>1.5011925383712628</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.681702384611031</c:v>
+                  <c:v>2.3138346280301421</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.191150689039841</c:v>
+                  <c:v>-2.2739465732144191</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.004013849921265</c:v>
+                  <c:v>-9.2447734437237568</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.579694473720835</c:v>
+                  <c:v>-15.916502689127183</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.708799095622027</c:v>
+                  <c:v>-22.766081677568749</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.786368185588906</c:v>
+                  <c:v>-28.449452686153165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41.627533640903927</c:v>
+                  <c:v>-28.449452686153172</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45.117228869596609</c:v>
+                  <c:v>-26.948260147781916</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44.101785852867266</c:v>
+                  <c:v>-26.13561805812304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.433558039669059</c:v>
+                  <c:v>-24.800563196540597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3774,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3827,8 +3826,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>180/7</f>
-        <v>25.714285714285715</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -3837,7 +3835,8 @@
         <v>60</v>
       </c>
       <c r="D2">
-        <v>67.53994047895678</v>
+        <f>2.67*180/PI()</f>
+        <v>152.9797312999298</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3946,23 +3945,23 @@
       </c>
       <c r="G5">
         <f>SIN(PI()*($D$2+(F5-3)*$A$2)/180)</f>
-        <v>0.92414607390473669</v>
+        <v>0.45430566983030646</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H14" si="1">$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G5)*(ABS(G5))^($E$5+$C$8*($E$8-$E$5))</f>
-        <v>134.97592702454676</v>
+        <v>105.38361849839781</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I14" si="2">I4+(H5-$B$5)</f>
-        <v>41.975927024546763</v>
+        <f>I4+(H5-$B$5)</f>
+        <v>12.383618498397809</v>
       </c>
       <c r="J5">
         <f>J4+$A$5*COS(PI()*I5/180)</f>
-        <v>27.203981278266617</v>
+        <v>28.837135435453831</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K14" si="3">K4+$A$5*SIN(PI()*I5/180)</f>
-        <v>4.6817281911117554</v>
+        <f t="shared" ref="K5:K14" si="2">K4+$A$5*SIN(PI()*I5/180)</f>
+        <v>1.5011925383712628</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3972,23 +3971,23 @@
       </c>
       <c r="G6">
         <f>SIN(PI()*($D$2+(F6-3)*$A$2)/180)</f>
-        <v>0.99838748612542505</v>
+        <v>-0.3086805335240469</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>140.8684931415562</v>
+        <v>87.282979693398588</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
-        <v>89.844420166102964</v>
+        <f t="shared" ref="I5:I14" si="3">I5+(H6-$B$5)</f>
+        <v>6.6665981917963961</v>
       </c>
       <c r="J6">
         <f>J5+$A$5*COS(PI()*I6/180)</f>
-        <v>27.222988917366919</v>
+        <v>35.789804910850663</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>11.681702384611031</v>
+        <f t="shared" si="2"/>
+        <v>2.3138346280301421</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4004,28 +4003,28 @@
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G14" si="4">SIN(PI()*($D$2+(F7-3)*$A$2)/180)</f>
-        <v>0.87488601229999619</v>
+        <v>-0.89084586678057642</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>131.24359775093944</v>
+        <v>45.383618498397809</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>128.08801791704241</v>
+        <f t="shared" si="3"/>
+        <v>-40.949783309805795</v>
       </c>
       <c r="J7">
         <f>J6+$A$5*COS(PI()*I7/180)</f>
-        <v>22.904889870236744</v>
+        <v>41.07679494767757</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>17.191150689039841</v>
+        <f t="shared" si="2"/>
+        <v>-2.2739465732144191</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -4036,23 +4035,23 @@
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>0.57810263396575434</v>
+        <v>-0.95116577326106011</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>111.90817656860636</v>
+        <v>38.717020306601377</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
-        <v>146.99619448564877</v>
+        <f t="shared" si="3"/>
+        <v>-95.232763003204411</v>
       </c>
       <c r="J8">
         <f t="shared" ref="J8:J13" si="5">J7+$A$5*COS(PI()*I8/180)</f>
-        <v>17.034449127294753</v>
+        <v>40.43838070802984</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>21.004013849921265</v>
+        <f t="shared" si="2"/>
+        <v>-9.2447734437237568</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4062,23 +4061,23 @@
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>0.16681893901106776</v>
+        <v>-0.45430566983030735</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>95.28590585685582</v>
+        <v>80.616381501602149</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>149.28210034250458</v>
+        <f t="shared" si="3"/>
+        <v>-107.61638150160226</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>11.01660000351437</v>
+        <v>38.319883864504078</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>24.579694473720835</v>
+        <f t="shared" si="2"/>
+        <v>-15.916502689127183</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -4088,23 +4087,23 @@
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>-0.27750529271478519</v>
+        <v>0.30868053352404595</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>87.569967894277681</v>
+        <v>98.717020306601384</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>143.85206823678226</v>
+        <f t="shared" si="3"/>
+        <v>-101.89936119500088</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>5.3641231109128418</v>
+        <v>36.876530934310011</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>28.708799095622027</v>
+        <f t="shared" si="2"/>
+        <v>-22.766081677568749</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -4114,23 +4113,23 @@
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>-0.66686619783940693</v>
+        <v>0.89084586678057642</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>68.895005601270114</v>
+        <v>140.61638150160218</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>119.74707383805237</v>
+        <f t="shared" si="3"/>
+        <v>-54.282979693398701</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>1.8909179691627664</v>
+        <v>40.963007898491036</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>34.786368185588906</v>
+        <f t="shared" si="2"/>
+        <v>-28.449452686153165</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -4140,23 +4139,23 @@
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>-0.92414607390473658</v>
+        <v>0.95116577326106011</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>51.024072975453265</v>
+        <v>147.28297969339863</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
-        <v>77.771146813505638</v>
+        <f t="shared" si="3"/>
+        <v>-7.1054273576010019E-14</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>3.3736368275457087</v>
+        <v>47.963007898491036</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>41.627533640903927</v>
+        <f t="shared" si="2"/>
+        <v>-28.449452686153172</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -4166,23 +4165,23 @@
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>-0.99838748612542505</v>
+        <v>0.45430566983030668</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>45.131506858443792</v>
+        <v>105.38361849839782</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>29.90265367194943</v>
+        <f t="shared" si="3"/>
+        <v>12.383618498397752</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>9.4417524502773258</v>
+        <v>54.800143333944867</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>45.117228869596609</v>
+        <f t="shared" si="2"/>
+        <v>-26.948260147781916</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -4192,23 +4191,23 @@
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>-0.87488601229999585</v>
+        <v>-0.30868053352404584</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>54.756402249060564</v>
+        <v>87.28297969339863</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>-8.340944078990006</v>
+        <f t="shared" si="3"/>
+        <v>6.6665981917963819</v>
       </c>
       <c r="J14">
         <f>J13+$A$5*COS(PI()*I14/180)</f>
-        <v>16.367709097540981</v>
+        <v>61.752812809341698</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>44.101785852867266</v>
+        <f t="shared" si="2"/>
+        <v>-26.13561805812304</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -4225,71 +4224,79 @@
       </c>
       <c r="I15">
         <f>I14+(H15-$B$5)</f>
-        <v>-8.340944078990006</v>
+        <v>6.6665981917963819</v>
       </c>
       <c r="J15">
         <f>J14+$D$5*COS(PI()*I15/180)</f>
-        <v>27.746066446616986</v>
+        <v>73.175055518922207</v>
       </c>
       <c r="K15">
         <f>K14+$D$5*SIN(PI()*I15/180)</f>
-        <v>42.433558039669059</v>
+        <v>-24.800563196540597</v>
       </c>
       <c r="L15">
         <f>K15/J15</f>
-        <v>1.5293540120834996</v>
+        <v>-0.33892100280166459</v>
       </c>
       <c r="M15">
         <f>SLOPE(K3:K14, J3:J14)</f>
-        <v>-1.2750929103360547</v>
+        <v>-0.74310593621491472</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>180*ATAN(M15)/PI()</f>
-        <v>-51.894450498809817</v>
-      </c>
-    </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-36.616259484833911</v>
+      </c>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f>133*PI()/180</f>
+        <v>2.3212879051524582</v>
+      </c>
       <c r="J17">
         <f>AVERAGE(J2:J15)</f>
-        <v>14.754793935624003</v>
+        <v>38.356611304286915</v>
       </c>
       <c r="K17">
         <f>AVERAGE(K2:K15)</f>
-        <v>22.565254519475179</v>
+        <v>-12.940687427998899</v>
       </c>
       <c r="L17">
         <f>K17-L15*J17</f>
-        <v>-4.8783436678689895E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="10:12" x14ac:dyDescent="0.25">
+        <v>5.9173739323686192E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>46.38*PI()/180</f>
+        <v>0.80948370707496997</v>
+      </c>
       <c r="K19">
         <f>SLOPE(K2:K15, F2:F15)/SLOPE(J2:J15,F2:F15)</f>
-        <v>-20.751888894693302</v>
-      </c>
-    </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-0.67376541408369162</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K22">
         <v>-10</v>
       </c>
       <c r="L22">
         <f>$L$15*K22</f>
-        <v>-15.293540120834997</v>
-      </c>
-    </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+        <v>3.3892100280166462</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K23">
         <f>K22+5</f>
         <v>-5</v>
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L50" si="6">$L$15*K23</f>
-        <v>-7.6467700604174986</v>
-      </c>
-    </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+        <v>1.6946050140083231</v>
+      </c>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K24">
         <f t="shared" ref="K24:K27" si="7">K23+5</f>
         <v>0</v>
@@ -4299,84 +4306,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K25">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L25">
         <f t="shared" si="6"/>
-        <v>7.6467700604174986</v>
-      </c>
-    </row>
-    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-1.6946050140083231</v>
+      </c>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K26">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="L26">
         <f t="shared" si="6"/>
-        <v>15.293540120834997</v>
-      </c>
-    </row>
-    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-3.3892100280166462</v>
+      </c>
+    </row>
+    <row r="27" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K27">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="L27">
         <f t="shared" si="6"/>
-        <v>22.940310181252496</v>
-      </c>
-    </row>
-    <row r="28" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-5.0838150420249688</v>
+      </c>
+    </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K28">
         <f>K27+5</f>
         <v>20</v>
       </c>
       <c r="L28">
         <f t="shared" si="6"/>
-        <v>30.587080241669995</v>
-      </c>
-    </row>
-    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-6.7784200560332923</v>
+      </c>
+    </row>
+    <row r="29" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K29">
         <f t="shared" ref="K29:K50" si="8">K28+5</f>
         <v>25</v>
       </c>
       <c r="L29">
         <f t="shared" si="6"/>
-        <v>38.23385030208749</v>
-      </c>
-    </row>
-    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-8.473025070041615</v>
+      </c>
+    </row>
+    <row r="30" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K30">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="L30">
         <f t="shared" si="6"/>
-        <v>45.880620362504992</v>
-      </c>
-    </row>
-    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-10.167630084049938</v>
+      </c>
+    </row>
+    <row r="31" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K31">
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="L31">
         <f t="shared" si="6"/>
-        <v>53.527390422922487</v>
-      </c>
-    </row>
-    <row r="32" spans="10:12" x14ac:dyDescent="0.25">
+        <v>-11.86223509805826</v>
+      </c>
+    </row>
+    <row r="32" spans="7:12" x14ac:dyDescent="0.25">
       <c r="K32">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="L32">
         <f t="shared" si="6"/>
-        <v>61.174160483339989</v>
+        <v>-13.556840112066585</v>
       </c>
     </row>
     <row r="33" spans="11:12" x14ac:dyDescent="0.25">
@@ -4386,7 +4393,7 @@
       </c>
       <c r="L33">
         <f t="shared" si="6"/>
-        <v>68.820930543757484</v>
+        <v>-15.251445126074907</v>
       </c>
     </row>
     <row r="34" spans="11:12" x14ac:dyDescent="0.25">
@@ -4396,7 +4403,7 @@
       </c>
       <c r="L34">
         <f t="shared" si="6"/>
-        <v>76.467700604174979</v>
+        <v>-16.94605014008323</v>
       </c>
     </row>
     <row r="35" spans="11:12" x14ac:dyDescent="0.25">
@@ -4406,7 +4413,7 @@
       </c>
       <c r="L35">
         <f t="shared" si="6"/>
-        <v>84.114470664592474</v>
+        <v>-18.640655154091554</v>
       </c>
     </row>
     <row r="36" spans="11:12" x14ac:dyDescent="0.25">
@@ -4416,7 +4423,7 @@
       </c>
       <c r="L36">
         <f t="shared" si="6"/>
-        <v>91.761240725009984</v>
+        <v>-20.335260168099875</v>
       </c>
     </row>
     <row r="37" spans="11:12" x14ac:dyDescent="0.25">
@@ -4426,7 +4433,7 @@
       </c>
       <c r="L37">
         <f t="shared" si="6"/>
-        <v>99.408010785427479</v>
+        <v>-22.0298651821082</v>
       </c>
     </row>
     <row r="38" spans="11:12" x14ac:dyDescent="0.25">
@@ -4436,7 +4443,7 @@
       </c>
       <c r="L38">
         <f t="shared" si="6"/>
-        <v>107.05478084584497</v>
+        <v>-23.724470196116521</v>
       </c>
     </row>
     <row r="39" spans="11:12" x14ac:dyDescent="0.25">
@@ -4446,7 +4453,7 @@
       </c>
       <c r="L39">
         <f t="shared" si="6"/>
-        <v>114.70155090626247</v>
+        <v>-25.419075210124845</v>
       </c>
     </row>
     <row r="40" spans="11:12" x14ac:dyDescent="0.25">
@@ -4456,7 +4463,7 @@
       </c>
       <c r="L40">
         <f t="shared" si="6"/>
-        <v>122.34832096667998</v>
+        <v>-27.113680224133169</v>
       </c>
     </row>
     <row r="41" spans="11:12" x14ac:dyDescent="0.25">
@@ -4466,7 +4473,7 @@
       </c>
       <c r="L41">
         <f t="shared" si="6"/>
-        <v>129.99509102709746</v>
+        <v>-28.80828523814149</v>
       </c>
     </row>
     <row r="42" spans="11:12" x14ac:dyDescent="0.25">
@@ -4476,7 +4483,7 @@
       </c>
       <c r="L42">
         <f t="shared" si="6"/>
-        <v>137.64186108751497</v>
+        <v>-30.502890252149815</v>
       </c>
     </row>
     <row r="43" spans="11:12" x14ac:dyDescent="0.25">
@@ -4486,7 +4493,7 @@
       </c>
       <c r="L43">
         <f t="shared" si="6"/>
-        <v>145.28863114793248</v>
+        <v>-32.197495266158136</v>
       </c>
     </row>
     <row r="44" spans="11:12" x14ac:dyDescent="0.25">
@@ -4496,7 +4503,7 @@
       </c>
       <c r="L44">
         <f t="shared" si="6"/>
-        <v>152.93540120834996</v>
+        <v>-33.89210028016646</v>
       </c>
     </row>
     <row r="45" spans="11:12" x14ac:dyDescent="0.25">
@@ -4506,7 +4513,7 @@
       </c>
       <c r="L45">
         <f t="shared" si="6"/>
-        <v>160.58217126876747</v>
+        <v>-35.586705294174784</v>
       </c>
     </row>
     <row r="46" spans="11:12" x14ac:dyDescent="0.25">
@@ -4516,7 +4523,7 @@
       </c>
       <c r="L46">
         <f t="shared" si="6"/>
-        <v>168.22894132918495</v>
+        <v>-37.281310308183109</v>
       </c>
     </row>
     <row r="47" spans="11:12" x14ac:dyDescent="0.25">
@@ -4526,7 +4533,7 @@
       </c>
       <c r="L47">
         <f t="shared" si="6"/>
-        <v>175.87571138960246</v>
+        <v>-38.975915322191426</v>
       </c>
     </row>
     <row r="48" spans="11:12" x14ac:dyDescent="0.25">
@@ -4536,7 +4543,7 @@
       </c>
       <c r="L48">
         <f t="shared" si="6"/>
-        <v>183.52248145001997</v>
+        <v>-40.67052033619975</v>
       </c>
     </row>
     <row r="49" spans="11:12" x14ac:dyDescent="0.25">
@@ -4546,7 +4553,7 @@
       </c>
       <c r="L49">
         <f t="shared" si="6"/>
-        <v>191.16925151043745</v>
+        <v>-42.365125350208075</v>
       </c>
     </row>
     <row r="50" spans="11:12" x14ac:dyDescent="0.25">
@@ -4556,7 +4563,7 @@
       </c>
       <c r="L50">
         <f t="shared" si="6"/>
-        <v>198.81602157085496</v>
+        <v>-44.059730364216399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix and improve installer batch script, refactor concertina motion sketch, and add concertina demo sketch
Added "/Q" switch to "DEL" command in installer batch script and support
for predefined Arduino install paths (located in
"predefined_install_paths.txt" and currently consisting of the Penn
State lab install location). The concertina motion sketch was
refactored: concertina motion calculations were moved to library header
files. A concertina demonstration sketch ("ConcertinaMotionDemo") was
added that also depends on these library header files.
</commit_message>
<xml_diff>
--- a/Concertina Wave Calculator.xlsx
+++ b/Concertina Wave Calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\My Documents\GitHub\SnakeRobot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\My Documents\SnakeRobot - 4-11-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -215,43 +215,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.837135435453831</c:v>
+                  <c:v>26.384882697190651</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.789804910850663</c:v>
+                  <c:v>26.379055036553098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.07679494767757</c:v>
+                  <c:v>20.678607957773522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.43838070802984</c:v>
+                  <c:v>13.75127718889685</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.319883864504078</c:v>
+                  <c:v>6.7837924943551853</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.876530934310011</c:v>
+                  <c:v>-8.6448353836917846E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.963007898491036</c:v>
+                  <c:v>-5.1357798992726922</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47.963007898491036</c:v>
+                  <c:v>-3.7884979528288092</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.800143333944867</c:v>
+                  <c:v>2.5848888690502054</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>61.752812809341698</c:v>
+                  <c:v>9.5766142866756461</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73.175055518922207</c:v>
+                  <c:v>21.063020329917443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -272,37 +272,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5011925383712628</c:v>
+                  <c:v>3.7905350071337001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3138346280301421</c:v>
+                  <c:v>10.790532581302671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.2739465732144191</c:v>
+                  <c:v>14.853155268931122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.2447734437237568</c:v>
+                  <c:v>15.859181321563227</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-15.916502689127183</c:v>
+                  <c:v>16.533093060092572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22.766081677568749</c:v>
+                  <c:v>17.874655838285474</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-28.449452686153165</c:v>
+                  <c:v>22.722774127298973</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-28.449452686153172</c:v>
+                  <c:v>29.591895712828403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-26.948260147781916</c:v>
+                  <c:v>32.486708387026667</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-26.13561805812304</c:v>
+                  <c:v>32.146450125509986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-24.800563196540597</c:v>
+                  <c:v>31.587454410161151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,7 +349,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>38.356611304286915</c:v>
+                  <c:v>10.870815189605297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,7 +361,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-12.940687427998899</c:v>
+                  <c:v>16.302602560009568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -504,91 +504,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>3.3892100280166462</c:v>
+                  <c:v>-14.996640517549631</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6946050140083231</c:v>
+                  <c:v>-7.4983202587748154</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.6946050140083231</c:v>
+                  <c:v>7.4983202587748154</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.3892100280166462</c:v>
+                  <c:v>14.996640517549631</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.0838150420249688</c:v>
+                  <c:v>22.494960776324447</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6.7784200560332923</c:v>
+                  <c:v>29.993281035099262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8.473025070041615</c:v>
+                  <c:v>37.491601293874076</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-10.167630084049938</c:v>
+                  <c:v>44.989921552648894</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-11.86223509805826</c:v>
+                  <c:v>52.488241811423705</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-13.556840112066585</c:v>
+                  <c:v>59.986562070198524</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-15.251445126074907</c:v>
+                  <c:v>67.484882328973342</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-16.94605014008323</c:v>
+                  <c:v>74.983202587748153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-18.640655154091554</c:v>
+                  <c:v>82.481522846522964</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-20.335260168099875</c:v>
+                  <c:v>89.979843105297789</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-22.0298651821082</c:v>
+                  <c:v>97.4781633640726</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-23.724470196116521</c:v>
+                  <c:v>104.97648362284741</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-25.419075210124845</c:v>
+                  <c:v>112.47480388162224</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-27.113680224133169</c:v>
+                  <c:v>119.97312414039705</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-28.80828523814149</c:v>
+                  <c:v>127.47144439917186</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-30.502890252149815</c:v>
+                  <c:v>134.96976465794668</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-32.197495266158136</c:v>
+                  <c:v>142.46808491672149</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-33.89210028016646</c:v>
+                  <c:v>149.96640517549631</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-35.586705294174784</c:v>
+                  <c:v>157.46472543427112</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-37.281310308183109</c:v>
+                  <c:v>164.96304569304593</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-38.975915322191426</c:v>
+                  <c:v>172.46136595182077</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-40.67052033619975</c:v>
+                  <c:v>179.95968621059558</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-42.365125350208075</c:v>
+                  <c:v>187.45800646937039</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-44.059730364216399</c:v>
+                  <c:v>194.9563267281452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1092,43 +1092,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.837135435453831</c:v>
+                  <c:v>26.384882697190651</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.789804910850663</c:v>
+                  <c:v>26.379055036553098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.07679494767757</c:v>
+                  <c:v>20.678607957773522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.43838070802984</c:v>
+                  <c:v>13.75127718889685</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.319883864504078</c:v>
+                  <c:v>6.7837924943551853</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.876530934310011</c:v>
+                  <c:v>-8.6448353836917846E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.963007898491036</c:v>
+                  <c:v>-5.1357798992726922</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47.963007898491036</c:v>
+                  <c:v>-3.7884979528288092</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.800143333944867</c:v>
+                  <c:v>2.5848888690502054</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>61.752812809341698</c:v>
+                  <c:v>9.5766142866756461</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73.175055518922207</c:v>
+                  <c:v>21.063020329917443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1523,37 +1523,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5011925383712628</c:v>
+                  <c:v>3.7905350071337001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3138346280301421</c:v>
+                  <c:v>10.790532581302671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.2739465732144191</c:v>
+                  <c:v>14.853155268931122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.2447734437237568</c:v>
+                  <c:v>15.859181321563227</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-15.916502689127183</c:v>
+                  <c:v>16.533093060092572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22.766081677568749</c:v>
+                  <c:v>17.874655838285474</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-28.449452686153165</c:v>
+                  <c:v>22.722774127298973</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-28.449452686153172</c:v>
+                  <c:v>29.591895712828403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-26.948260147781916</c:v>
+                  <c:v>32.486708387026667</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-26.13561805812304</c:v>
+                  <c:v>32.146450125509986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-24.800563196540597</c:v>
+                  <c:v>31.587454410161151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3773,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -3835,11 +3835,10 @@
         <v>60</v>
       </c>
       <c r="D2">
-        <f>2.67*180/PI()</f>
-        <v>152.9797312999298</v>
+        <v>47.664416515956525</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3877,7 +3876,7 @@
       </c>
       <c r="J3">
         <f>$E$2</f>
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3916,7 +3915,7 @@
       </c>
       <c r="J4">
         <f>J3+$A$5*COS(PI()*I4/180)</f>
-        <v>22</v>
+        <v>20.5</v>
       </c>
       <c r="K4">
         <f>K3+$A$5*SIN(PI()*I4/180)</f>
@@ -3945,23 +3944,23 @@
       </c>
       <c r="G5">
         <f>SIN(PI()*($D$2+(F5-3)*$A$2)/180)</f>
-        <v>0.45430566983030646</v>
+        <v>0.73921297864814284</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H14" si="1">$C$5+($B$2+$C$8*($C$2-$B$2))*SIGN(G5)*(ABS(G5))^($E$5+$C$8*($E$8-$E$5))</f>
-        <v>105.38361849839781</v>
+        <v>125.78614966811159</v>
       </c>
       <c r="I5">
         <f>I4+(H5-$B$5)</f>
-        <v>12.383618498397809</v>
+        <v>32.786149668111591</v>
       </c>
       <c r="J5">
         <f>J4+$A$5*COS(PI()*I5/180)</f>
-        <v>28.837135435453831</v>
+        <v>26.384882697190651</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K14" si="2">K4+$A$5*SIN(PI()*I5/180)</f>
-        <v>1.5011925383712628</v>
+        <v>3.7905350071337001</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3971,23 +3970,23 @@
       </c>
       <c r="G6">
         <f>SIN(PI()*($D$2+(F6-3)*$A$2)/180)</f>
-        <v>-0.3086805335240469</v>
+        <v>0.97691308372068464</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>87.282979693398588</v>
+        <v>150.26155038867944</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I5:I14" si="3">I5+(H6-$B$5)</f>
-        <v>6.6665981917963961</v>
+        <f t="shared" ref="I6:I14" si="3">I5+(H6-$B$5)</f>
+        <v>90.04770005679103</v>
       </c>
       <c r="J6">
         <f>J5+$A$5*COS(PI()*I6/180)</f>
-        <v>35.789804910850663</v>
+        <v>26.379055036553098</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>2.3138346280301421</v>
+        <v>10.790532581302671</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4003,23 +4002,23 @@
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G14" si="4">SIN(PI()*($D$2+(F7-3)*$A$2)/180)</f>
-        <v>-0.89084586678057642</v>
+        <v>0.95285011693487109</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>45.383618498397809</v>
+        <v>147.47540072056785</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>-40.949783309805795</v>
+        <v>144.52310077735888</v>
       </c>
       <c r="J7">
         <f>J6+$A$5*COS(PI()*I7/180)</f>
-        <v>41.07679494767757</v>
+        <v>20.678607957773522</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>-2.2739465732144191</v>
+        <v>14.853155268931122</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4035,23 +4034,23 @@
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>-0.95116577326106011</v>
+        <v>0.6734717308084579</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>38.717020306601377</v>
+        <v>120.21385033188839</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>-95.232763003204411</v>
+        <v>171.73695110924729</v>
       </c>
       <c r="J8">
         <f t="shared" ref="J8:J13" si="5">J7+$A$5*COS(PI()*I8/180)</f>
-        <v>40.43838070802984</v>
+        <v>13.75127718889685</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>-9.2447734437237568</v>
+        <v>15.859181321563227</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4061,23 +4060,23 @@
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>-0.45430566983030735</v>
+        <v>0.21363713828672809</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>80.616381501602149</v>
+        <v>95.738449611320561</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>-107.61638150160226</v>
+        <v>174.47540072056785</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>38.319883864504078</v>
+        <v>6.7837924943551853</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>-15.916502689127183</v>
+        <v>16.533093060092572</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -4087,23 +4086,23 @@
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>0.30868053352404595</v>
+        <v>-0.3034413529122269</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>98.717020306601384</v>
+        <v>87.475400720567848</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>-101.89936119500088</v>
+        <v>168.9508014411357</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>36.876530934310011</v>
+        <v>-8.6448353836917846E-2</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>-22.766081677568749</v>
+        <v>17.874655838285474</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -4113,23 +4112,23 @@
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>0.89084586678057642</v>
+        <v>-0.73921297864814273</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>140.61638150160218</v>
+        <v>60.21385033188843</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>-54.282979693398701</v>
+        <v>136.16465177302413</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>40.963007898491036</v>
+        <v>-5.1357798992726922</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>-28.449452686153165</v>
+        <v>22.722774127298973</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -4139,23 +4138,23 @@
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>0.95116577326106011</v>
+        <v>-0.97691308372068453</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>147.28297969339863</v>
+        <v>35.738449611320576</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>-7.1054273576010019E-14</v>
+        <v>78.903101384344708</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>47.963007898491036</v>
+        <v>-3.7884979528288092</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>-28.449452686153172</v>
+        <v>29.591895712828403</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -4165,23 +4164,23 @@
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>0.45430566983030668</v>
+        <v>-0.95285011693487121</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>105.38361849839782</v>
+        <v>38.524599279432138</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>12.383618498397752</v>
+        <v>24.427700663776847</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>54.800143333944867</v>
+        <v>2.5848888690502054</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>-26.948260147781916</v>
+        <v>32.486708387026667</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -4191,23 +4190,23 @@
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>-0.30868053352404584</v>
+        <v>-0.6734717308084579</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>87.28297969339863</v>
+        <v>65.786149668111605</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>6.6665981917963819</v>
+        <v>-2.7861496681115483</v>
       </c>
       <c r="J14">
         <f>J13+$A$5*COS(PI()*I14/180)</f>
-        <v>61.752812809341698</v>
+        <v>9.5766142866756461</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>-26.13561805812304</v>
+        <v>32.146450125509986</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -4224,29 +4223,29 @@
       </c>
       <c r="I15">
         <f>I14+(H15-$B$5)</f>
-        <v>6.6665981917963819</v>
+        <v>-2.7861496681115483</v>
       </c>
       <c r="J15">
         <f>J14+$D$5*COS(PI()*I15/180)</f>
-        <v>73.175055518922207</v>
+        <v>21.063020329917443</v>
       </c>
       <c r="K15">
         <f>K14+$D$5*SIN(PI()*I15/180)</f>
-        <v>-24.800563196540597</v>
+        <v>31.587454410161151</v>
       </c>
       <c r="L15">
         <f>K15/J15</f>
-        <v>-0.33892100280166459</v>
+        <v>1.4996640517549631</v>
       </c>
       <c r="M15">
         <f>SLOPE(K3:K14, J3:J14)</f>
-        <v>-0.74310593621491472</v>
+        <v>-0.70799648199781073</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>180*ATAN(M15)/PI()</f>
-        <v>-36.616259484833911</v>
+        <v>-35.298359499202988</v>
       </c>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
@@ -4256,15 +4255,15 @@
       </c>
       <c r="J17">
         <f>AVERAGE(J2:J15)</f>
-        <v>38.356611304286915</v>
+        <v>10.870815189605297</v>
       </c>
       <c r="K17">
         <f>AVERAGE(K2:K15)</f>
-        <v>-12.940687427998899</v>
+        <v>16.302602560009568</v>
       </c>
       <c r="L17">
         <f>K17-L15*J17</f>
-        <v>5.9173739323686192E-2</v>
+        <v>3.1806886688912073E-5</v>
       </c>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
@@ -4274,7 +4273,7 @@
       </c>
       <c r="K19">
         <f>SLOPE(K2:K15, F2:F15)/SLOPE(J2:J15,F2:F15)</f>
-        <v>-0.67376541408369162</v>
+        <v>-3.544630053070835</v>
       </c>
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.25">
@@ -4283,7 +4282,7 @@
       </c>
       <c r="L22">
         <f>$L$15*K22</f>
-        <v>3.3892100280166462</v>
+        <v>-14.996640517549631</v>
       </c>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.25">
@@ -4293,7 +4292,7 @@
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L50" si="6">$L$15*K23</f>
-        <v>1.6946050140083231</v>
+        <v>-7.4983202587748154</v>
       </c>
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.25">
@@ -4313,7 +4312,7 @@
       </c>
       <c r="L25">
         <f t="shared" si="6"/>
-        <v>-1.6946050140083231</v>
+        <v>7.4983202587748154</v>
       </c>
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.25">
@@ -4323,7 +4322,7 @@
       </c>
       <c r="L26">
         <f t="shared" si="6"/>
-        <v>-3.3892100280166462</v>
+        <v>14.996640517549631</v>
       </c>
     </row>
     <row r="27" spans="7:12" x14ac:dyDescent="0.25">
@@ -4333,7 +4332,7 @@
       </c>
       <c r="L27">
         <f t="shared" si="6"/>
-        <v>-5.0838150420249688</v>
+        <v>22.494960776324447</v>
       </c>
     </row>
     <row r="28" spans="7:12" x14ac:dyDescent="0.25">
@@ -4343,7 +4342,7 @@
       </c>
       <c r="L28">
         <f t="shared" si="6"/>
-        <v>-6.7784200560332923</v>
+        <v>29.993281035099262</v>
       </c>
     </row>
     <row r="29" spans="7:12" x14ac:dyDescent="0.25">
@@ -4353,7 +4352,7 @@
       </c>
       <c r="L29">
         <f t="shared" si="6"/>
-        <v>-8.473025070041615</v>
+        <v>37.491601293874076</v>
       </c>
     </row>
     <row r="30" spans="7:12" x14ac:dyDescent="0.25">
@@ -4363,7 +4362,7 @@
       </c>
       <c r="L30">
         <f t="shared" si="6"/>
-        <v>-10.167630084049938</v>
+        <v>44.989921552648894</v>
       </c>
     </row>
     <row r="31" spans="7:12" x14ac:dyDescent="0.25">
@@ -4373,7 +4372,7 @@
       </c>
       <c r="L31">
         <f t="shared" si="6"/>
-        <v>-11.86223509805826</v>
+        <v>52.488241811423705</v>
       </c>
     </row>
     <row r="32" spans="7:12" x14ac:dyDescent="0.25">
@@ -4383,7 +4382,7 @@
       </c>
       <c r="L32">
         <f t="shared" si="6"/>
-        <v>-13.556840112066585</v>
+        <v>59.986562070198524</v>
       </c>
     </row>
     <row r="33" spans="11:12" x14ac:dyDescent="0.25">
@@ -4393,7 +4392,7 @@
       </c>
       <c r="L33">
         <f t="shared" si="6"/>
-        <v>-15.251445126074907</v>
+        <v>67.484882328973342</v>
       </c>
     </row>
     <row r="34" spans="11:12" x14ac:dyDescent="0.25">
@@ -4403,7 +4402,7 @@
       </c>
       <c r="L34">
         <f t="shared" si="6"/>
-        <v>-16.94605014008323</v>
+        <v>74.983202587748153</v>
       </c>
     </row>
     <row r="35" spans="11:12" x14ac:dyDescent="0.25">
@@ -4413,7 +4412,7 @@
       </c>
       <c r="L35">
         <f t="shared" si="6"/>
-        <v>-18.640655154091554</v>
+        <v>82.481522846522964</v>
       </c>
     </row>
     <row r="36" spans="11:12" x14ac:dyDescent="0.25">
@@ -4423,7 +4422,7 @@
       </c>
       <c r="L36">
         <f t="shared" si="6"/>
-        <v>-20.335260168099875</v>
+        <v>89.979843105297789</v>
       </c>
     </row>
     <row r="37" spans="11:12" x14ac:dyDescent="0.25">
@@ -4433,7 +4432,7 @@
       </c>
       <c r="L37">
         <f t="shared" si="6"/>
-        <v>-22.0298651821082</v>
+        <v>97.4781633640726</v>
       </c>
     </row>
     <row r="38" spans="11:12" x14ac:dyDescent="0.25">
@@ -4443,7 +4442,7 @@
       </c>
       <c r="L38">
         <f t="shared" si="6"/>
-        <v>-23.724470196116521</v>
+        <v>104.97648362284741</v>
       </c>
     </row>
     <row r="39" spans="11:12" x14ac:dyDescent="0.25">
@@ -4453,7 +4452,7 @@
       </c>
       <c r="L39">
         <f t="shared" si="6"/>
-        <v>-25.419075210124845</v>
+        <v>112.47480388162224</v>
       </c>
     </row>
     <row r="40" spans="11:12" x14ac:dyDescent="0.25">
@@ -4463,7 +4462,7 @@
       </c>
       <c r="L40">
         <f t="shared" si="6"/>
-        <v>-27.113680224133169</v>
+        <v>119.97312414039705</v>
       </c>
     </row>
     <row r="41" spans="11:12" x14ac:dyDescent="0.25">
@@ -4473,7 +4472,7 @@
       </c>
       <c r="L41">
         <f t="shared" si="6"/>
-        <v>-28.80828523814149</v>
+        <v>127.47144439917186</v>
       </c>
     </row>
     <row r="42" spans="11:12" x14ac:dyDescent="0.25">
@@ -4483,7 +4482,7 @@
       </c>
       <c r="L42">
         <f t="shared" si="6"/>
-        <v>-30.502890252149815</v>
+        <v>134.96976465794668</v>
       </c>
     </row>
     <row r="43" spans="11:12" x14ac:dyDescent="0.25">
@@ -4493,7 +4492,7 @@
       </c>
       <c r="L43">
         <f t="shared" si="6"/>
-        <v>-32.197495266158136</v>
+        <v>142.46808491672149</v>
       </c>
     </row>
     <row r="44" spans="11:12" x14ac:dyDescent="0.25">
@@ -4503,7 +4502,7 @@
       </c>
       <c r="L44">
         <f t="shared" si="6"/>
-        <v>-33.89210028016646</v>
+        <v>149.96640517549631</v>
       </c>
     </row>
     <row r="45" spans="11:12" x14ac:dyDescent="0.25">
@@ -4513,7 +4512,7 @@
       </c>
       <c r="L45">
         <f t="shared" si="6"/>
-        <v>-35.586705294174784</v>
+        <v>157.46472543427112</v>
       </c>
     </row>
     <row r="46" spans="11:12" x14ac:dyDescent="0.25">
@@ -4523,7 +4522,7 @@
       </c>
       <c r="L46">
         <f t="shared" si="6"/>
-        <v>-37.281310308183109</v>
+        <v>164.96304569304593</v>
       </c>
     </row>
     <row r="47" spans="11:12" x14ac:dyDescent="0.25">
@@ -4533,7 +4532,7 @@
       </c>
       <c r="L47">
         <f t="shared" si="6"/>
-        <v>-38.975915322191426</v>
+        <v>172.46136595182077</v>
       </c>
     </row>
     <row r="48" spans="11:12" x14ac:dyDescent="0.25">
@@ -4543,7 +4542,7 @@
       </c>
       <c r="L48">
         <f t="shared" si="6"/>
-        <v>-40.67052033619975</v>
+        <v>179.95968621059558</v>
       </c>
     </row>
     <row r="49" spans="11:12" x14ac:dyDescent="0.25">
@@ -4553,7 +4552,7 @@
       </c>
       <c r="L49">
         <f t="shared" si="6"/>
-        <v>-42.365125350208075</v>
+        <v>187.45800646937039</v>
       </c>
     </row>
     <row r="50" spans="11:12" x14ac:dyDescent="0.25">
@@ -4563,7 +4562,7 @@
       </c>
       <c r="L50">
         <f t="shared" si="6"/>
-        <v>-44.059730364216399</v>
+        <v>194.9563267281452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>